<commit_message>
Cleaned things up, added batteryMassModel, fixed battery cell selection
</commit_message>
<xml_diff>
--- a/Lists/ComboList&Data.xlsx
+++ b/Lists/ComboList&Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" state="visible" r:id="rId2"/>
@@ -409,11 +409,11 @@
   </sheetPr>
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G64" activeCellId="0" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -2723,7 +2723,7 @@
       <selection pane="topLeft" activeCell="B854" activeCellId="0" sqref="B854"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -16004,7 +16004,7 @@
       <selection pane="topLeft" activeCell="F864" activeCellId="0" sqref="F864"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -31952,11 +31952,11 @@
   </sheetPr>
   <dimension ref="A1:G365"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A327" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A318" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G322" activeCellId="0" sqref="G322"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -37198,11 +37198,11 @@
   </sheetPr>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.28"/>

</xml_diff>

<commit_message>
Made some examples for UMD
</commit_message>
<xml_diff>
--- a/Lists/ComboList&Data.xlsx
+++ b/Lists/ComboList&Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="98">
   <si>
     <t xml:space="preserve">Motor</t>
   </si>
@@ -250,6 +250,24 @@
     <t xml:space="preserve">TM-U13-KV100</t>
   </si>
   <si>
+    <t xml:space="preserve">KDE2315XF-885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9” x 3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9" x 4.5 (DJI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10" x 3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11" x 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12” x 4.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Voltage</t>
   </si>
   <si>
@@ -423,17 +441,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G122" activeCellId="0" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
@@ -3132,6 +3150,126 @@
         <v>80</v>
       </c>
       <c r="G117" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <v>17000</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <f aca="false">75+10</f>
+        <v>85</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G118" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <v>17000</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <f aca="false">75+10</f>
+        <v>85</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G119" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <f aca="false">75+10</f>
+        <v>85</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G120" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <v>11000</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <f aca="false">75+10</f>
+        <v>85</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G121" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <f aca="false">75+10</f>
+        <v>85</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G122" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3147,17 +3285,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1030"/>
+  <dimension ref="A1:G1107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A487" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F514" activeCellId="0" sqref="F514"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1065" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1073" activeCellId="0" sqref="C1073"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -3172,22 +3310,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19085,6 +19223,1183 @@
       </c>
       <c r="G1030" s="0" t="n">
         <v>8560</v>
+      </c>
+    </row>
+    <row r="1031" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1031" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1031" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="C1031" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1031" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1031" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1031" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G1031" s="0" t="n">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="1032" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1032" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1032" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1032" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G1032" s="0" t="n">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="1033" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1033" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1033" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1033" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="G1033" s="0" t="n">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="1034" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1034" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1034" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F1034" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="G1034" s="0" t="n">
+        <v>6660</v>
+      </c>
+    </row>
+    <row r="1035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1035" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1035" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="F1035" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="G1035" s="0" t="n">
+        <v>7860</v>
+      </c>
+    </row>
+    <row r="1036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1036" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1036" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="F1036" s="0" t="n">
+        <v>610</v>
+      </c>
+      <c r="G1036" s="0" t="n">
+        <v>9060</v>
+      </c>
+    </row>
+    <row r="1037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1037" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1037" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="F1037" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="G1037" s="0" t="n">
+        <v>9960</v>
+      </c>
+    </row>
+    <row r="1038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1038" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1038" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="C1038" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1038" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1038" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1038" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="G1038" s="0" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="1039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1039" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1039" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1039" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="G1039" s="0" t="n">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="1040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1040" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1040" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1040" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="G1040" s="0" t="n">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="1041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1041" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1041" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="F1041" s="0" t="n">
+        <v>480</v>
+      </c>
+      <c r="G1041" s="0" t="n">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="1042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1042" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1042" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="F1042" s="0" t="n">
+        <v>640</v>
+      </c>
+      <c r="G1042" s="0" t="n">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="1043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1043" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1043" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="F1043" s="0" t="n">
+        <v>820</v>
+      </c>
+      <c r="G1043" s="0" t="n">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="1044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1044" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1044" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="F1044" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="G1044" s="0" t="n">
+        <v>8940</v>
+      </c>
+    </row>
+    <row r="1045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1045" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1045" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="C1045" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1045" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1045" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1045" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="G1045" s="0" t="n">
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="1046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1046" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1046" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1046" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="G1046" s="0" t="n">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="1047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1047" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1047" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1047" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G1047" s="0" t="n">
+        <v>5340</v>
+      </c>
+    </row>
+    <row r="1048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1048" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1048" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1048" s="0" t="n">
+        <v>430</v>
+      </c>
+      <c r="G1048" s="0" t="n">
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="1049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1049" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1049" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1049" s="0" t="n">
+        <v>590</v>
+      </c>
+      <c r="G1049" s="0" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="1050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1050" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1050" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="F1050" s="0" t="n">
+        <v>770</v>
+      </c>
+      <c r="G1050" s="0" t="n">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="1051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1051" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1051" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="F1051" s="0" t="n">
+        <v>940</v>
+      </c>
+      <c r="G1051" s="0" t="n">
+        <v>9480</v>
+      </c>
+    </row>
+    <row r="1052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1052" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1052" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="C1052" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1052" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1052" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1052" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="G1052" s="0" t="n">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="1053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1053" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1053" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1053" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="G1053" s="0" t="n">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="1054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1054" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1054" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1054" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G1054" s="0" t="n">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="1055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1055" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1055" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="F1055" s="0" t="n">
+        <v>570</v>
+      </c>
+      <c r="G1055" s="0" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="1056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1056" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1056" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="F1056" s="0" t="n">
+        <v>760</v>
+      </c>
+      <c r="G1056" s="0" t="n">
+        <v>6960</v>
+      </c>
+    </row>
+    <row r="1057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1057" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1057" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="F1057" s="0" t="n">
+        <v>990</v>
+      </c>
+      <c r="G1057" s="0" t="n">
+        <v>7860</v>
+      </c>
+    </row>
+    <row r="1058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1058" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1058" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="F1058" s="0" t="n">
+        <v>1170</v>
+      </c>
+      <c r="G1058" s="0" t="n">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="1059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1059" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1059" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="C1059" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1059" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1059" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1059" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="G1059" s="0" t="n">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="1060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1060" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1060" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1060" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="G1060" s="0" t="n">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="1061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1061" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1061" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1061" s="0" t="n">
+        <v>480</v>
+      </c>
+      <c r="G1061" s="0" t="n">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="1062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1062" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1062" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="F1062" s="0" t="n">
+        <v>670</v>
+      </c>
+      <c r="G1062" s="0" t="n">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="1063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1063" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1063" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="F1063" s="0" t="n">
+        <v>880</v>
+      </c>
+      <c r="G1063" s="0" t="n">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="1064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1064" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1064" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="F1064" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G1064" s="0" t="n">
+        <v>7020</v>
+      </c>
+    </row>
+    <row r="1065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1065" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1065" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="F1065" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="G1065" s="0" t="n">
+        <v>7560</v>
+      </c>
+    </row>
+    <row r="1066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1066" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C1066" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1066" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1066" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1066" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="G1066" s="0" t="n">
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="1067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1067" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1067" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1067" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="G1067" s="0" t="n">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="1068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1068" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1068" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="F1068" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="G1068" s="0" t="n">
+        <v>7140</v>
+      </c>
+    </row>
+    <row r="1069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1069" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1069" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="F1069" s="0" t="n">
+        <v>540</v>
+      </c>
+      <c r="G1069" s="0" t="n">
+        <v>8520</v>
+      </c>
+    </row>
+    <row r="1070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1070" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1070" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="F1070" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="G1070" s="0" t="n">
+        <v>9980</v>
+      </c>
+    </row>
+    <row r="1071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1071" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1071" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="F1071" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="G1071" s="0" t="n">
+        <v>11480</v>
+      </c>
+    </row>
+    <row r="1072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1072" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1072" s="0" t="n">
+        <v>232</v>
+      </c>
+      <c r="F1072" s="0" t="n">
+        <v>1160</v>
+      </c>
+      <c r="G1072" s="0" t="n">
+        <v>12420</v>
+      </c>
+    </row>
+    <row r="1073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1073" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1073" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C1073" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1073" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1073" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1073" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="G1073" s="0" t="n">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="1074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1074" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1074" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="F1074" s="0" t="n">
+        <v>320</v>
+      </c>
+      <c r="G1074" s="0" t="n">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="1075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1075" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1075" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="F1075" s="0" t="n">
+        <v>510</v>
+      </c>
+      <c r="G1075" s="0" t="n">
+        <v>6420</v>
+      </c>
+    </row>
+    <row r="1076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1076" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1076" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="F1076" s="0" t="n">
+        <v>730</v>
+      </c>
+      <c r="G1076" s="0" t="n">
+        <v>7740</v>
+      </c>
+    </row>
+    <row r="1077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1077" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1077" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="F1077" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="G1077" s="0" t="n">
+        <v>8910</v>
+      </c>
+    </row>
+    <row r="1078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1078" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1078" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="F1078" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="G1078" s="0" t="n">
+        <v>9960</v>
+      </c>
+    </row>
+    <row r="1079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1079" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1079" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="F1079" s="0" t="n">
+        <v>1440</v>
+      </c>
+      <c r="G1079" s="0" t="n">
+        <v>10920</v>
+      </c>
+    </row>
+    <row r="1080" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1080" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1080" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C1080" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1080" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1080" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1080" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="G1080" s="0" t="n">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="1081" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1081" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1081" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1081" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="G1081" s="0" t="n">
+        <v>5220</v>
+      </c>
+    </row>
+    <row r="1082" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1082" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1082" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="F1082" s="0" t="n">
+        <v>470</v>
+      </c>
+      <c r="G1082" s="0" t="n">
+        <v>6720</v>
+      </c>
+    </row>
+    <row r="1083" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1083" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1083" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1083" s="0" t="n">
+        <v>690</v>
+      </c>
+      <c r="G1083" s="0" t="n">
+        <v>8180</v>
+      </c>
+    </row>
+    <row r="1084" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1084" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1084" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="F1084" s="0" t="n">
+        <v>920</v>
+      </c>
+      <c r="G1084" s="0" t="n">
+        <v>9360</v>
+      </c>
+    </row>
+    <row r="1085" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1085" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1085" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="F1085" s="0" t="n">
+        <v>1210</v>
+      </c>
+      <c r="G1085" s="0" t="n">
+        <v>10680</v>
+      </c>
+    </row>
+    <row r="1086" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1086" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1086" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="F1086" s="0" t="n">
+        <v>1430</v>
+      </c>
+      <c r="G1086" s="0" t="n">
+        <v>11640</v>
+      </c>
+    </row>
+    <row r="1087" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1087" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1087" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C1087" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1087" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1087" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1087" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="G1087" s="0" t="n">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="1088" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1088" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1088" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1088" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="G1088" s="0" t="n">
+        <v>4860</v>
+      </c>
+    </row>
+    <row r="1089" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1089" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1089" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="F1089" s="0" t="n">
+        <v>610</v>
+      </c>
+      <c r="G1089" s="0" t="n">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="1090" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1090" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1090" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="F1090" s="0" t="n">
+        <v>870</v>
+      </c>
+      <c r="G1090" s="0" t="n">
+        <v>7380</v>
+      </c>
+    </row>
+    <row r="1091" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1091" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1091" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="F1091" s="0" t="n">
+        <v>1160</v>
+      </c>
+      <c r="G1091" s="0" t="n">
+        <v>8520</v>
+      </c>
+    </row>
+    <row r="1092" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1092" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1092" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="F1092" s="0" t="n">
+        <v>1440</v>
+      </c>
+      <c r="G1092" s="0" t="n">
+        <v>9480</v>
+      </c>
+    </row>
+    <row r="1093" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1093" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1093" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="F1093" s="0" t="n">
+        <v>1650</v>
+      </c>
+      <c r="G1093" s="0" t="n">
+        <v>10320</v>
+      </c>
+    </row>
+    <row r="1094" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1094" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1094" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C1094" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1094" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1094" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1094" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="G1094" s="0" t="n">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="1095" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1095" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1095" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F1095" s="0" t="n">
+        <v>440</v>
+      </c>
+      <c r="G1095" s="0" t="n">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="1096" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1096" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1096" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="F1096" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="G1096" s="0" t="n">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="1097" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1097" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1097" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="F1097" s="0" t="n">
+        <v>980</v>
+      </c>
+      <c r="G1097" s="0" t="n">
+        <v>6660</v>
+      </c>
+    </row>
+    <row r="1098" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1098" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1098" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="F1098" s="0" t="n">
+        <v>1260</v>
+      </c>
+      <c r="G1098" s="0" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="1099" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1099" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1099" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="F1099" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G1099" s="0" t="n">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="1100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1100" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1100" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="F1100" s="0" t="n">
+        <v>1820</v>
+      </c>
+      <c r="G1100" s="0" t="n">
+        <v>9040</v>
+      </c>
+    </row>
+    <row r="1101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1101" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1101" s="0" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="C1101" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1101" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E1101" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F1101" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="G1101" s="0" t="n">
+        <v>5460</v>
+      </c>
+    </row>
+    <row r="1102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1102" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E1102" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="F1102" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="G1102" s="0" t="n">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="1103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1103" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1103" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="F1103" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="G1103" s="0" t="n">
+        <v>9720</v>
+      </c>
+    </row>
+    <row r="1104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1104" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E1104" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="F1104" s="0" t="n">
+        <v>1030</v>
+      </c>
+      <c r="G1104" s="0" t="n">
+        <v>11640</v>
+      </c>
+    </row>
+    <row r="1105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1105" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E1105" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="F1105" s="0" t="n">
+        <v>1390</v>
+      </c>
+      <c r="G1105" s="0" t="n">
+        <v>13440</v>
+      </c>
+    </row>
+    <row r="1106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1106" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E1106" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="F1106" s="0" t="n">
+        <v>1760</v>
+      </c>
+      <c r="G1106" s="0" t="n">
+        <v>15060</v>
+      </c>
+    </row>
+    <row r="1107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1107" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1107" s="0" t="n">
+        <v>605</v>
+      </c>
+      <c r="F1107" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G1107" s="0" t="n">
+        <v>16260</v>
       </c>
     </row>
   </sheetData>
@@ -19099,7 +20414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -19109,7 +20424,7 @@
       <selection pane="topLeft" activeCell="G114" activeCellId="0" sqref="G114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -19121,22 +20436,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19263,7 +20578,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>187.2</v>
@@ -19278,7 +20593,7 @@
     <row r="10" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="D10" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>235.2</v>
@@ -19293,7 +20608,7 @@
     <row r="11" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="D11" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>292.8</v>
@@ -19308,7 +20623,7 @@
     <row r="12" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="D12" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>360</v>
@@ -19323,7 +20638,7 @@
     <row r="13" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="D13" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>518.4</v>
@@ -19338,7 +20653,7 @@
     <row r="14" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="D14" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>720</v>
@@ -19353,7 +20668,7 @@
     <row r="15" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="D15" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1080</v>
@@ -19376,7 +20691,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>206.4</v>
@@ -19391,7 +20706,7 @@
     <row r="17" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="D17" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>264</v>
@@ -19406,7 +20721,7 @@
     <row r="18" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="D18" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>350.4</v>
@@ -19421,7 +20736,7 @@
     <row r="19" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="D19" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>422.4</v>
@@ -19436,7 +20751,7 @@
     <row r="20" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="D20" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>600</v>
@@ -19451,7 +20766,7 @@
     <row r="21" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="D21" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>820.8</v>
@@ -19466,7 +20781,7 @@
     <row r="22" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="D22" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1219.2</v>
@@ -19489,7 +20804,7 @@
         <v>62</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>240</v>
@@ -19504,7 +20819,7 @@
     <row r="24" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="D24" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>316.8</v>
@@ -19519,7 +20834,7 @@
     <row r="25" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="D25" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>398.4</v>
@@ -19534,7 +20849,7 @@
     <row r="26" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="D26" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>480</v>
@@ -19549,7 +20864,7 @@
     <row r="27" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="D27" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>662.4</v>
@@ -19564,7 +20879,7 @@
     <row r="28" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="D28" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>926.4</v>
@@ -19579,7 +20894,7 @@
     <row r="29" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="D29" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>1425.6</v>
@@ -19602,7 +20917,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>259.2</v>
@@ -19617,7 +20932,7 @@
     <row r="31" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="D31" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>345.6</v>
@@ -19632,7 +20947,7 @@
     <row r="32" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="D32" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>441.6</v>
@@ -19647,7 +20962,7 @@
     <row r="33" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="D33" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>552</v>
@@ -19662,7 +20977,7 @@
     <row r="34" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="D34" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>796.8</v>
@@ -19677,7 +20992,7 @@
     <row r="35" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="D35" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1080</v>
@@ -19692,7 +21007,7 @@
     <row r="36" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="D36" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1622.4</v>
@@ -19715,7 +21030,7 @@
         <v>63</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>164</v>
@@ -19730,7 +21045,7 @@
     <row r="38" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="D38" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>204</v>
@@ -19745,7 +21060,7 @@
     <row r="39" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="D39" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>268</v>
@@ -19760,7 +21075,7 @@
     <row r="40" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="D40" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>328</v>
@@ -19775,7 +21090,7 @@
     <row r="41" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="D41" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>484</v>
@@ -19790,7 +21105,7 @@
     <row r="42" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="D42" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>684</v>
@@ -19805,7 +21120,7 @@
     <row r="43" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="D43" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>992</v>
@@ -19828,7 +21143,7 @@
         <v>66</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>131.2</v>
@@ -19843,7 +21158,7 @@
     <row r="45" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="D45" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>172.8</v>
@@ -19858,7 +21173,7 @@
     <row r="46" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="D46" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>217.6</v>
@@ -19873,7 +21188,7 @@
     <row r="47" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="D47" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>2518</v>
@@ -19888,7 +21203,7 @@
     <row r="48" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="D48" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>374.4</v>
@@ -19903,7 +21218,7 @@
     <row r="49" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="D49" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>518.4</v>
@@ -19918,7 +21233,7 @@
     <row r="50" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
       <c r="D50" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>771.2</v>
@@ -19941,7 +21256,7 @@
         <v>64</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>156</v>
@@ -19956,7 +21271,7 @@
     <row r="52" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="D52" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>196</v>
@@ -19971,7 +21286,7 @@
     <row r="53" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="D53" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>244</v>
@@ -19986,7 +21301,7 @@
     <row r="54" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="D54" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>300</v>
@@ -20001,7 +21316,7 @@
     <row r="55" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
       <c r="D55" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>432</v>
@@ -20016,7 +21331,7 @@
     <row r="56" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
       <c r="D56" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>612</v>
@@ -20031,7 +21346,7 @@
     <row r="57" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
       <c r="D57" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>904</v>
@@ -20054,7 +21369,7 @@
         <v>65</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>184</v>
@@ -20069,7 +21384,7 @@
     <row r="59" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
       <c r="D59" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>236</v>
@@ -20084,7 +21399,7 @@
     <row r="60" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
       <c r="D60" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>304</v>
@@ -20099,7 +21414,7 @@
     <row r="61" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
       <c r="D61" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>372</v>
@@ -20114,7 +21429,7 @@
     <row r="62" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
       <c r="D62" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>540</v>
@@ -20129,7 +21444,7 @@
     <row r="63" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
       <c r="D63" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>756</v>
@@ -20144,7 +21459,7 @@
     <row r="64" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1"/>
       <c r="D64" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>1104</v>
@@ -20167,7 +21482,7 @@
         <v>66</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>228</v>
@@ -20182,7 +21497,7 @@
     <row r="66" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1"/>
       <c r="D66" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>296</v>
@@ -20197,7 +21512,7 @@
     <row r="67" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1"/>
       <c r="D67" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>368</v>
@@ -20212,7 +21527,7 @@
     <row r="68" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
       <c r="D68" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>468</v>
@@ -20227,7 +21542,7 @@
     <row r="69" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
       <c r="D69" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>668</v>
@@ -20242,7 +21557,7 @@
     <row r="70" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="D70" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>928</v>
@@ -20257,7 +21572,7 @@
     <row r="71" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
       <c r="D71" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>1348</v>
@@ -20280,7 +21595,7 @@
         <v>64</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>249.6</v>
@@ -20295,7 +21610,7 @@
     <row r="73" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
       <c r="D73" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>326.4</v>
@@ -20310,7 +21625,7 @@
     <row r="74" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1"/>
       <c r="D74" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>408</v>
@@ -20325,7 +21640,7 @@
     <row r="75" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
       <c r="D75" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>480</v>
@@ -20340,7 +21655,7 @@
     <row r="76" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1"/>
       <c r="D76" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>715.2</v>
@@ -20355,7 +21670,7 @@
     <row r="77" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1"/>
       <c r="D77" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>979.2</v>
@@ -20370,7 +21685,7 @@
     <row r="78" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1"/>
       <c r="D78" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>1478.4</v>
@@ -20393,7 +21708,7 @@
         <v>65</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>297.6</v>
@@ -20408,7 +21723,7 @@
     <row r="80" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
       <c r="D80" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>398.4</v>
@@ -20423,7 +21738,7 @@
     <row r="81" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
       <c r="D81" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>494.4</v>
@@ -20438,7 +21753,7 @@
     <row r="82" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
       <c r="D82" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>614.4</v>
@@ -20453,7 +21768,7 @@
     <row r="83" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1"/>
       <c r="D83" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>878.4</v>
@@ -20468,7 +21783,7 @@
     <row r="84" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1"/>
       <c r="D84" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>1171.2</v>
@@ -20483,7 +21798,7 @@
     <row r="85" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
       <c r="D85" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>1776</v>
@@ -26913,7 +28228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26923,7 +28238,7 @@
       <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.28"/>
@@ -26934,22 +28249,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26973,13 +28288,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>46.2</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>4</v>
@@ -27161,13 +28476,13 @@
         <v>0</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>46.2</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>4</v>
@@ -27361,13 +28676,13 @@
         <v>0</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>46.2</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>4</v>
@@ -27561,13 +28876,13 @@
         <v>0</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>46.2</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="K23" s="0" t="n">
         <v>2</v>
@@ -27761,13 +29076,13 @@
         <v>0</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>23.1</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="K30" s="0" t="n">
         <v>4</v>

</xml_diff>